<commit_message>
update new DB, please run .sql file
</commit_message>
<xml_diff>
--- a/config/Data-Model-Report.xlsx
+++ b/config/Data-Model-Report.xlsx
@@ -11,14 +11,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="munFJrZh5tOMWUdtqTa771RhIwaZ11VaKGYwTKdi96k="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="F7+OVw8I8PizCFa1eOr/2XzAFvZV0IR4C2z3SnaG3P8="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="102">
   <si>
     <t>Collumn</t>
   </si>
@@ -173,6 +173,30 @@
     <t>mentor_id</t>
   </si>
   <si>
+    <t>TeamMember</t>
+  </si>
+  <si>
+    <t>team_member_id</t>
+  </si>
+  <si>
+    <t>team_member_name</t>
+  </si>
+  <si>
+    <t>team_member_gender</t>
+  </si>
+  <si>
+    <t>VARCHAR(10)</t>
+  </si>
+  <si>
+    <t>Text_Gender</t>
+  </si>
+  <si>
+    <t>team_member_phone</t>
+  </si>
+  <si>
+    <t>team_id</t>
+  </si>
+  <si>
     <t>Location</t>
   </si>
   <si>
@@ -206,6 +230,15 @@
     <t>Text_Bus_Route_Back_ITZone</t>
   </si>
   <si>
+    <t>location_map</t>
+  </si>
+  <si>
+    <t>VARCHAR(1000)</t>
+  </si>
+  <si>
+    <t>Text_Iframe_Link</t>
+  </si>
+  <si>
     <t>member_id</t>
   </si>
   <si>
@@ -252,9 +285,6 @@
   </si>
   <si>
     <t>team_puzzle_id</t>
-  </si>
-  <si>
-    <t>team_id</t>
   </si>
   <si>
     <t>time_end</t>
@@ -332,7 +362,7 @@
       <patternFill patternType="lightGray"/>
     </fill>
   </fills>
-  <borders count="21">
+  <borders count="24">
     <border/>
     <border>
       <left style="thin">
@@ -551,6 +581,33 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -588,7 +645,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -654,6 +711,15 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="23" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -3511,16 +3577,16 @@
       </c>
     </row>
     <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="18" t="s">
+      <c r="C22" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="12" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="18" t="s">
@@ -3534,14 +3600,14 @@
       </c>
     </row>
     <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="11" t="s">
+      <c r="A23" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="23" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>23</v>
@@ -3557,14 +3623,14 @@
       </c>
     </row>
     <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="11" t="s">
+      <c r="A24" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>23</v>
@@ -3576,15 +3642,15 @@
         <v>25</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>56</v>
+      <c r="B25" s="23" t="s">
+        <v>57</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>22</v>
@@ -3599,110 +3665,110 @@
         <v>25</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="23" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1">
+      <c r="A27" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" ht="14.25" customHeight="1">
+      <c r="A28" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1">
+      <c r="A29" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D29" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B28" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="17" t="s">
+      <c r="E29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="13" t="s">
         <v>63</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F29" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="30" ht="14.25" customHeight="1">
       <c r="A30" s="11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>23</v>
@@ -3714,18 +3780,18 @@
         <v>25</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" ht="14.25" customHeight="1">
       <c r="A31" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B31" s="12" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>66</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D31" s="12" t="s">
         <v>23</v>
@@ -3736,19 +3802,19 @@
       <c r="F31" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>68</v>
+      <c r="G31" s="21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" ht="14.25" customHeight="1">
       <c r="A32" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="12" t="s">
-        <v>69</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="20" t="s">
+        <v>68</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>23</v>
@@ -3759,88 +3825,88 @@
       <c r="F32" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G32" s="13" t="s">
-        <v>57</v>
+      <c r="G32" s="21" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C33" s="15" t="s">
+      <c r="A33" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1">
+      <c r="A34" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D34" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="15" t="s">
+      <c r="E34" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G33" s="16" t="s">
+      <c r="G34" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="18" t="s">
+    <row r="35" ht="14.25" customHeight="1">
+      <c r="A35" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="18" t="s">
+      <c r="D35" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E34" s="18" t="s">
+      <c r="E35" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G34" s="19" t="s">
+      <c r="F35" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="19" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="13" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="B36" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="D36" s="12" t="s">
         <v>23</v>
@@ -3851,114 +3917,114 @@
       <c r="F36" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G36" s="21" t="s">
-        <v>75</v>
+      <c r="G36" s="13" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="15" t="s">
+      <c r="A37" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E37" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="15" t="s">
+      <c r="E37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1">
+      <c r="A38" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1">
+      <c r="A39" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="G37" s="16" t="s">
+      <c r="G39" s="16" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="C38" s="18" t="s">
+    <row r="40" ht="14.25" customHeight="1">
+      <c r="A40" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D38" s="18" t="s">
+      <c r="D40" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E38" s="18" t="s">
+      <c r="E40" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F38" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B39" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G39" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="13" t="s">
+      <c r="F40" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G40" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="41" ht="14.25" customHeight="1">
       <c r="A41" s="11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>80</v>
+        <v>48</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>25</v>
@@ -3967,84 +4033,84 @@
         <v>25</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>82</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" ht="14.25" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>84</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="D42" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" customHeight="1">
+      <c r="A43" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B43" s="23" t="s">
-        <v>84</v>
-      </c>
-      <c r="C43" s="23" t="s">
-        <v>74</v>
+      <c r="B43" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="15" t="s">
+        <v>22</v>
       </c>
       <c r="D43" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E43" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>85</v>
+      <c r="E43" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="G43" s="16" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="B44" s="9" t="s">
+      <c r="A44" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="C44" s="9" t="s">
+      <c r="B44" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D44" s="9" t="s">
+      <c r="D44" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E44" s="9" t="s">
+      <c r="E44" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="10" t="s">
+      <c r="F44" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="19" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="45" ht="14.25" customHeight="1">
       <c r="A45" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>22</v>
@@ -4064,10 +4130,10 @@
     </row>
     <row r="46" ht="14.25" customHeight="1">
       <c r="A46" s="11" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="C46" s="12" t="s">
         <v>22</v>
@@ -4087,65 +4153,197 @@
     </row>
     <row r="47" ht="14.25" customHeight="1">
       <c r="A47" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
+      </c>
+      <c r="B47" s="12" t="s">
+        <v>89</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="D47" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F47" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1">
+      <c r="A48" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D48" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="E48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F48" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25" customHeight="1">
+      <c r="A49" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="26" t="s">
+        <v>85</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="C48" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="D48" s="15" t="s">
+      <c r="E49" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F49" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25" customHeight="1">
+      <c r="A50" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E48" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="16" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-    </row>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
+      <c r="E50" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1">
+      <c r="A51" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D51" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F51" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25" customHeight="1">
+      <c r="A52" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F52" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25" customHeight="1">
+      <c r="A53" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="D53" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="21" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" ht="14.25" customHeight="1">
+      <c r="A54" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F54" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="16" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25" customHeight="1">
+      <c r="A55" s="28"/>
+      <c r="B55" s="28"/>
+      <c r="C55" s="28"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28"/>
+      <c r="G55" s="28"/>
+    </row>
     <row r="56" ht="14.25" customHeight="1"/>
     <row r="57" ht="14.25" customHeight="1"/>
     <row r="58" ht="14.25" customHeight="1"/>
@@ -5100,6 +5298,12 @@
     <row r="1007" ht="14.25" customHeight="1"/>
     <row r="1008" ht="14.25" customHeight="1"/>
     <row r="1009" ht="14.25" customHeight="1"/>
+    <row r="1010" ht="14.25" customHeight="1"/>
+    <row r="1011" ht="14.25" customHeight="1"/>
+    <row r="1012" ht="14.25" customHeight="1"/>
+    <row r="1013" ht="14.25" customHeight="1"/>
+    <row r="1014" ht="14.25" customHeight="1"/>
+    <row r="1015" ht="14.25" customHeight="1"/>
   </sheetData>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
update new DB and hint, please check carefully
</commit_message>
<xml_diff>
--- a/config/Data-Model-Report.xlsx
+++ b/config/Data-Model-Report.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
+  <bookViews>
+    <workbookView windowWidth="23040" windowHeight="9120" activeTab="2"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Collumn Meaning" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Example" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Data Model Report" sheetId="3" r:id="rId6"/>
+    <sheet name="Collumn Meaning" sheetId="1" r:id="rId1"/>
+    <sheet name="Example" sheetId="2" r:id="rId2"/>
+    <sheet name="Data Model Report" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId7" roundtripDataChecksum="F7+OVw8I8PizCFa1eOr/2XzAFvZV0IR4C2z3SnaG3P8="/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="107">
   <si>
     <t>Collumn</t>
   </si>
@@ -194,6 +205,18 @@
     <t>team_member_phone</t>
   </si>
   <si>
+    <t>is_team_leader</t>
+  </si>
+  <si>
+    <t>NUMBER(1)</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Number_Show_Is_Team_Leader</t>
+  </si>
+  <si>
     <t>team_id</t>
   </si>
   <si>
@@ -272,15 +295,27 @@
     <t>hint_description</t>
   </si>
   <si>
+    <t>hint_end</t>
+  </si>
+  <si>
+    <t>DATETIME</t>
+  </si>
+  <si>
+    <t>Datetime</t>
+  </si>
+  <si>
     <t>is_show</t>
   </si>
   <si>
-    <t>NUMBER(1)</t>
-  </si>
-  <si>
     <t>Number_Show_Hint_Status</t>
   </si>
   <si>
+    <t>hint_priority</t>
+  </si>
+  <si>
+    <t>Number_Show_Hint_Priority</t>
+  </si>
+  <si>
     <t>TeamPuzzle</t>
   </si>
   <si>
@@ -288,15 +323,6 @@
   </si>
   <si>
     <t>time_end</t>
-  </si>
-  <si>
-    <t>DATETIME</t>
-  </si>
-  <si>
-    <t>Null</t>
-  </si>
-  <si>
-    <t>Datetime</t>
   </si>
   <si>
     <t>time_fine</t>
@@ -329,54 +355,380 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="22">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="24">
-    <border/>
+  <borders count="34">
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -391,6 +743,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -405,6 +758,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -419,6 +773,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -427,9 +782,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -438,9 +795,11 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -449,9 +808,11 @@
       <right style="thick">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -466,12 +827,13 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thick">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
@@ -480,6 +842,22 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -494,6 +872,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -508,6 +887,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -522,6 +902,7 @@
       <bottom style="thick">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -536,6 +917,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -550,6 +932,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -564,6 +947,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -575,6 +959,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -586,6 +972,60 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thick">
@@ -594,151 +1034,607 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FFB2B2B2"/>
       </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color rgb="FF3F3F3F"/>
       </right>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="thick">
-        <color rgb="FF000000"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
-  </cellStyleXfs>
-  <cellXfs count="29">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellStyleXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="20" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="22" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="23" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+  </cellStyleXfs>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="double">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <left style="thin">
+          <color theme="4"/>
+        </left>
+        <right style="thin">
+          <color theme="4"/>
+        </right>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+        <horizontal style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1"/>
+      </font>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <border>
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <top style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="1"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.799981688894314"/>
+          <bgColor theme="4" tint="0.799981688894314"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="4" tint="0.399975585192419"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStylePreset3_Accent1" defaultPivotStyle="PivotStylePreset2_Accent1">
+    <tableStyle name="TableStylePreset3_Accent1" pivot="0" count="7" xr9:uid="{59DB682C-5494-4EDE-A608-00C9E5F0F923}">
+      <tableStyleElement type="wholeTable" dxfId="6"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="totalRow" dxfId="4"/>
+      <tableStyleElement type="firstColumn" dxfId="3"/>
+      <tableStyleElement type="lastColumn" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="0"/>
+    </tableStyle>
+    <tableStyle name="PivotStylePreset2_Accent1" table="0" count="10" xr9:uid="{267968C8-6FFD-4C36-ACC1-9EA1FD1885CA}">
+      <tableStyleElement type="headerRow" dxfId="16"/>
+      <tableStyleElement type="totalRow" dxfId="15"/>
+      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="12"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="11"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="10"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="9"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="8"/>
+      <tableStyleElement type="pageFieldValues" dxfId="7"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -749,16 +1645,20 @@
     <xdr:ext cx="9553575" cy="4162425"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Creating Data Model Report from erwin" id="0" name="image1.png"/>
+        <xdr:cNvPr id="2" name="image1.png" descr="Creating Data Model Report from erwin"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9553575" cy="4162425"/>
+        </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
@@ -770,12 +1670,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -965,85 +1861,87 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.71"/>
-    <col customWidth="1" min="2" max="2" width="79.71"/>
-    <col customWidth="1" min="3" max="26" width="8.71"/>
+    <col min="1" max="1" width="21.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="79.712962962963" customWidth="1"/>
+    <col min="3" max="26" width="8.71296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A3" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="27" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A4" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A5" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A6" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="14.25" customHeight="1" spans="1:2">
+      <c r="A7" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="27" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="28.8" spans="1:2">
+      <c r="A8" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="29" t="s">
         <v>15</v>
       </c>
     </row>
@@ -2040,30 +2938,30 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="landscape"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="32.71"/>
-    <col customWidth="1" min="2" max="2" width="33.86"/>
-    <col customWidth="1" min="3" max="3" width="16.86"/>
-    <col customWidth="1" min="4" max="4" width="11.14"/>
-    <col customWidth="1" min="5" max="5" width="14.71"/>
-    <col customWidth="1" min="6" max="6" width="33.71"/>
-    <col customWidth="1" min="7" max="26" width="8.71"/>
+    <col min="1" max="1" width="32.712962962963" customWidth="1"/>
+    <col min="2" max="2" width="33.8611111111111" customWidth="1"/>
+    <col min="3" max="3" width="16.8611111111111" customWidth="1"/>
+    <col min="4" max="4" width="11.1388888888889" customWidth="1"/>
+    <col min="5" max="5" width="14.712962962963" customWidth="1"/>
+    <col min="6" max="6" width="33.712962962963" customWidth="1"/>
+    <col min="7" max="26" width="8.71296296296296" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1"/>
@@ -3067,1285 +3965,1344 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup paperSize="1" orientation="landscape"/>
+  <headerFooter/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G1018"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="24.71"/>
-    <col customWidth="1" min="2" max="3" width="28.71"/>
-    <col customWidth="1" min="4" max="4" width="17.86"/>
-    <col customWidth="1" min="5" max="5" width="18.0"/>
-    <col customWidth="1" min="6" max="6" width="17.57"/>
-    <col customWidth="1" min="7" max="7" width="42.14"/>
-    <col customWidth="1" min="8" max="26" width="8.71"/>
+    <col min="1" max="1" width="24.712962962963" customWidth="1"/>
+    <col min="2" max="3" width="28.712962962963" customWidth="1"/>
+    <col min="4" max="4" width="17.8611111111111" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.5740740740741" customWidth="1"/>
+    <col min="7" max="7" width="42.1388888888889" customWidth="1"/>
+    <col min="8" max="26" width="8.71296296296296" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="2" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" s="10" t="s">
+      <c r="F2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" s="11" t="s">
+    <row r="3" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A3" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="10" t="s">
+      <c r="E3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="11" t="s">
+    <row r="4" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" s="13" t="s">
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="11" t="s">
+    <row r="5" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="13" t="s">
+      <c r="G5" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="14" t="s">
+    <row r="6" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="15" t="s">
+      <c r="E6" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="17" t="s">
+    <row r="7" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A7" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="E7" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="F7" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="14" t="s">
+    <row r="8" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A8" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" s="16" t="s">
+      <c r="E8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="17" t="s">
+    <row r="9" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A9" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="18" t="s">
+      <c r="D9" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="11" t="s">
+    <row r="10" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="E10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="14" t="s">
+    <row r="11" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A11" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="16" t="s">
+      <c r="E11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="17" t="s">
+    <row r="12" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="18" t="s">
+      <c r="B12" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" s="19" t="s">
+      <c r="F12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="11" t="s">
+    <row r="13" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="13" t="s">
+      <c r="E13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="11" t="s">
+    <row r="14" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A14" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="13" t="s">
+      <c r="E14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G14" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="14" t="s">
+    <row r="15" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A15" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="16" t="s">
+      <c r="E15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="17" t="s">
+    <row r="16" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A16" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="18" t="s">
+      <c r="E16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G16" s="19" t="s">
+      <c r="F16" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="11" t="s">
+    <row r="17" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="12" t="s">
+      <c r="B17" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="13" t="s">
+      <c r="E17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="11" t="s">
+    <row r="18" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G18" s="13" t="s">
+      <c r="E18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="11" t="s">
+    <row r="19" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="13" t="s">
+      <c r="E19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="11" t="s">
+    <row r="20" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" s="21" t="s">
+      <c r="E20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" s="17" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="14" t="s">
+    <row r="21" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A21" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G21" s="16" t="s">
+      <c r="G21" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="22" t="s">
+    <row r="22" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A22" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="23" t="s">
+      <c r="B22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="18" t="s">
+      <c r="E22" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G22" s="19" t="s">
+      <c r="F22" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="22" t="s">
+    <row r="23" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" s="13" t="s">
+      <c r="E23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="22" t="s">
+    <row r="24" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A24" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="13" t="s">
+      <c r="E24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="22" t="s">
+    <row r="25" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A25" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E25" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="13" t="s">
+      <c r="E25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="22" t="s">
+    <row r="26" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A26" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A27" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="15" t="s">
+      <c r="E27" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G27" s="12" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="17" t="s">
+    <row r="28" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A28" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="33" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A34" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A35" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A36" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A37" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A38" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A40" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A41" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A42" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A43" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A44" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="D44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A45" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A46" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A47" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E47" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F47" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G47" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A48" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A49" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A50" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D50" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C27" s="18" t="s">
+      <c r="E50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A51" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="52" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A52" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B52" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C52" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A53" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D53" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="18" t="s">
+      <c r="E53" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G27" s="19" t="s">
+      <c r="F53" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="11" t="s">
+    <row r="54" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A54" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A55" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G55" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A56" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="B28" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="12" t="s">
+      <c r="D56" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G28" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="11" t="s">
+      <c r="E56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G56" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="57" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A57" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D29" s="12" t="s">
+      <c r="D57" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G29" s="13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D30" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" ht="14.25" customHeight="1">
-      <c r="A31" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" ht="14.25" customHeight="1">
-      <c r="A32" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G32" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" ht="14.25" customHeight="1">
-      <c r="A33" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G33" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="34" ht="14.25" customHeight="1">
-      <c r="A34" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G34" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" ht="14.25" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D35" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E35" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="37" ht="14.25" customHeight="1">
-      <c r="A37" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G37" s="13" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" ht="14.25" customHeight="1">
-      <c r="A38" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B38" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" ht="14.25" customHeight="1">
-      <c r="A39" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="B39" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G39" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" ht="14.25" customHeight="1">
-      <c r="A40" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="B40" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D40" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E40" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" ht="14.25" customHeight="1">
-      <c r="A41" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G41" s="13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" ht="14.25" customHeight="1">
-      <c r="A42" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G42" s="21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="43" ht="14.25" customHeight="1">
-      <c r="A43" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="B43" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C43" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E43" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F43" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G43" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="44" ht="14.25" customHeight="1">
-      <c r="A44" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="B44" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="18" t="s">
-        <v>24</v>
-      </c>
-      <c r="F44" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" ht="14.25" customHeight="1">
-      <c r="A45" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E45" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F45" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G45" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="46" ht="14.25" customHeight="1">
-      <c r="A46" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B46" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E46" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F46" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G46" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" ht="14.25" customHeight="1">
-      <c r="A47" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B47" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C47" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D47" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="48" ht="14.25" customHeight="1">
-      <c r="A48" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="C48" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="E48" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F48" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G48" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="49" ht="14.25" customHeight="1">
-      <c r="A49" s="25" t="s">
-        <v>87</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>94</v>
-      </c>
-      <c r="C49" s="26" t="s">
-        <v>85</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E49" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="F49" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="G49" s="27" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="50" ht="14.25" customHeight="1">
-      <c r="A50" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" ht="14.25" customHeight="1">
-      <c r="A51" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="C51" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E51" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F51" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G51" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" ht="14.25" customHeight="1">
-      <c r="A52" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D52" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F52" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" ht="14.25" customHeight="1">
-      <c r="A53" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C53" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D53" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E53" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="F53" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1">
-      <c r="A54" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="C54" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F54" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="55" ht="14.25" customHeight="1">
-      <c r="A55" s="28"/>
-      <c r="B55" s="28"/>
-      <c r="C55" s="28"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="28"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="28"/>
-    </row>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
+      <c r="E57" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="12" t="s">
+        <v>106</v>
+      </c>
+    </row>
     <row r="58" ht="14.25" customHeight="1"/>
     <row r="59" ht="14.25" customHeight="1"/>
     <row r="60" ht="14.25" customHeight="1"/>
@@ -5304,10 +6261,12 @@
     <row r="1013" ht="14.25" customHeight="1"/>
     <row r="1014" ht="14.25" customHeight="1"/>
     <row r="1015" ht="14.25" customHeight="1"/>
+    <row r="1016" ht="14.25" customHeight="1"/>
+    <row r="1017" ht="14.25" customHeight="1"/>
+    <row r="1018" ht="14.25" customHeight="1"/>
   </sheetData>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update new DB, page effect function and support question FE, please check carefully and import .sql file to mysql
</commit_message>
<xml_diff>
--- a/config/Data-Model-Report.xlsx
+++ b/config/Data-Model-Report.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="109">
   <si>
     <t>Collumn</t>
   </si>
@@ -326,6 +326,12 @@
   </si>
   <si>
     <t>time_fine</t>
+  </si>
+  <si>
+    <t>is_done</t>
+  </si>
+  <si>
+    <t>Number_Show_Is_Team_Done_Challenge</t>
   </si>
   <si>
     <t>is_clicked_check</t>
@@ -722,7 +728,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1038,6 +1044,36 @@
         <color rgb="FF000000"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1197,7 +1233,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1209,34 +1245,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="28" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="32" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="29" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="31" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="33" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="32" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="34" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="35" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1321,7 +1357,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1348,6 +1384,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1882,66 +1920,66 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="29" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="29" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="29" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="29" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="29" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="1:2">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="31" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3975,10 +4013,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1018"/>
+  <dimension ref="A1:G1019"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
@@ -5166,80 +5204,80 @@
       </c>
     </row>
     <row r="52" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B52" s="24" t="s">
+      <c r="B52" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="24" t="s">
+      <c r="C52" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G52" s="24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="53" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A53" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="F52" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G52" s="25" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A53" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B53" s="5" t="s">
+      <c r="E53" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F53" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="G53" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="C53" s="5" t="s">
+    </row>
+    <row r="54" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A54" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E53" s="5" t="s">
+      <c r="E54" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="54" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A54" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B54" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D54" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E54" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F54" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G54" s="9" t="s">
+      <c r="F54" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="55" ht="14.25" customHeight="1" spans="1:7">
       <c r="A55" s="7" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" s="8" t="s">
         <v>22</v>
@@ -5259,51 +5297,73 @@
     </row>
     <row r="56" ht="14.25" customHeight="1" spans="1:7">
       <c r="A56" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="B56" s="16" t="s">
         <v>103</v>
       </c>
+      <c r="B56" s="8" t="s">
+        <v>64</v>
+      </c>
       <c r="C56" s="8" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="D56" s="8" t="s">
         <v>23</v>
       </c>
       <c r="E56" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F56" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G56" s="17" t="s">
-        <v>104</v>
+      <c r="G56" s="9" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="57" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A57" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="B57" s="11" t="s">
+      <c r="A57" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B57" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D57" s="11" t="s">
+      <c r="D57" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E57" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F57" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G57" s="12" t="s">
+      <c r="E57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57" s="17" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A58" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B58" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D58" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>108</v>
+      </c>
+    </row>
     <row r="59" ht="14.25" customHeight="1"/>
     <row r="60" ht="14.25" customHeight="1"/>
     <row r="61" ht="14.25" customHeight="1"/>
@@ -6264,6 +6324,7 @@
     <row r="1016" ht="14.25" customHeight="1"/>
     <row r="1017" ht="14.25" customHeight="1"/>
     <row r="1018" ht="14.25" customHeight="1"/>
+    <row r="1019" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
update new DB, guard can open next location for team
</commit_message>
<xml_diff>
--- a/config/Data-Model-Report.xlsx
+++ b/config/Data-Model-Report.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="111">
   <si>
     <t>Collumn</t>
   </si>
@@ -350,6 +350,12 @@
   </si>
   <si>
     <t>Number_Show_Team_Arrival_Priority_In_Order</t>
+  </si>
+  <si>
+    <t>is_open_next_location</t>
+  </si>
+  <si>
+    <t>Number_Check_Is_Guard_Open_Next_Location</t>
   </si>
   <si>
     <t>is_show_next_location</t>
@@ -1357,7 +1363,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1386,6 +1392,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1920,66 +1927,66 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="30" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="30" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="14.25" customHeight="1" spans="1:2">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="28.8" spans="1:2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="32" t="s">
         <v>15</v>
       </c>
     </row>
@@ -4013,10 +4020,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G1019"/>
+  <dimension ref="A1:G1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4259259259259" defaultRowHeight="15" customHeight="1" outlineLevelCol="6"/>
@@ -5342,29 +5349,51 @@
       </c>
     </row>
     <row r="58" ht="14.25" customHeight="1" spans="1:7">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F58" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="12" t="s">
+      <c r="E58" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G58" s="17" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1" spans="1:7">
+      <c r="A59" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>110</v>
+      </c>
+    </row>
     <row r="60" ht="14.25" customHeight="1"/>
     <row r="61" ht="14.25" customHeight="1"/>
     <row r="62" ht="14.25" customHeight="1"/>
@@ -6325,6 +6354,7 @@
     <row r="1017" ht="14.25" customHeight="1"/>
     <row r="1018" ht="14.25" customHeight="1"/>
     <row r="1019" ht="14.25" customHeight="1"/>
+    <row r="1020" ht="14.25" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>